<commit_message>
problem statements updated in the workout file
</commit_message>
<xml_diff>
--- a/excel-beginner-tutorial_workout.xlsx
+++ b/excel-beginner-tutorial_workout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Projects\microsoft-excel-tutorial-beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB0CA13-D2D5-4F22-90B6-D563F5ACDF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD33637-6043-471D-9937-36240C535E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{9FA7835E-DA76-4B93-946E-CCC2848369CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="7" activeTab="15" xr2:uid="{9FA7835E-DA76-4B93-946E-CCC2848369CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="956">
   <si>
     <t>Reg No.</t>
   </si>
@@ -2603,9 +2603,6 @@
     <t>William.Gietz@company.com</t>
   </si>
   <si>
-    <t>Department</t>
-  </si>
-  <si>
     <t>=find()</t>
   </si>
   <si>
@@ -2655,6 +2652,300 @@
   </si>
   <si>
     <t>23:17:40</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Reg No</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Velma</t>
+  </si>
+  <si>
+    <t>Clemons</t>
+  </si>
+  <si>
+    <t>Kibo</t>
+  </si>
+  <si>
+    <t>Underwood</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Mcgee</t>
+  </si>
+  <si>
+    <t>Phyllis</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Zenaida</t>
+  </si>
+  <si>
+    <t>Decker</t>
+  </si>
+  <si>
+    <t>Gillian</t>
+  </si>
+  <si>
+    <t>Tillman</t>
+  </si>
+  <si>
+    <t>Constance</t>
+  </si>
+  <si>
+    <t>Boone</t>
+  </si>
+  <si>
+    <t>Giselle</t>
+  </si>
+  <si>
+    <t>Lancaster</t>
+  </si>
+  <si>
+    <t>Kirsten</t>
+  </si>
+  <si>
+    <t>Mcdowell</t>
+  </si>
+  <si>
+    <t>Solomon</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>Merrill</t>
+  </si>
+  <si>
+    <t>Carney</t>
+  </si>
+  <si>
+    <t>Hakeem</t>
+  </si>
+  <si>
+    <t>Gillespie</t>
+  </si>
+  <si>
+    <t>Hayden</t>
+  </si>
+  <si>
+    <t>Boyer</t>
+  </si>
+  <si>
+    <t>Griffin</t>
+  </si>
+  <si>
+    <t>Mcleod</t>
+  </si>
+  <si>
+    <t>Allistair</t>
+  </si>
+  <si>
+    <t>Patton</t>
+  </si>
+  <si>
+    <t>Rina</t>
+  </si>
+  <si>
+    <t>Slater</t>
+  </si>
+  <si>
+    <t>Caldwell</t>
+  </si>
+  <si>
+    <t>Skinner</t>
+  </si>
+  <si>
+    <t>Portia</t>
+  </si>
+  <si>
+    <t>Galloway</t>
+  </si>
+  <si>
+    <t>Noelle</t>
+  </si>
+  <si>
+    <t>Valentine</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>Petty</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>Fuller</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>Quinn</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Marcia</t>
+  </si>
+  <si>
+    <t>Shepard</t>
+  </si>
+  <si>
+    <t>Kieran</t>
+  </si>
+  <si>
+    <t>Moody</t>
+  </si>
+  <si>
+    <t>Brielle</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Jerome</t>
+  </si>
+  <si>
+    <t>Buckley</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Foreman</t>
+  </si>
+  <si>
+    <t>Gisela</t>
+  </si>
+  <si>
+    <t>Robertson</t>
+  </si>
+  <si>
+    <t>Sylvia</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>Madden</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Herman</t>
+  </si>
+  <si>
+    <t>Cora</t>
+  </si>
+  <si>
+    <t>Frazier</t>
+  </si>
+  <si>
+    <t>Yolanda</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Hadassah</t>
+  </si>
+  <si>
+    <t>Lowe</t>
+  </si>
+  <si>
+    <t>Ingrid</t>
+  </si>
+  <si>
+    <t>Yang</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Spence</t>
+  </si>
+  <si>
+    <t>Iola</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Kitra</t>
+  </si>
+  <si>
+    <t>Sparks</t>
+  </si>
+  <si>
+    <t>Carly</t>
+  </si>
+  <si>
+    <t>Bray</t>
+  </si>
+  <si>
+    <t>Leilani</t>
+  </si>
+  <si>
+    <t>Beard</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Bowen</t>
+  </si>
+  <si>
+    <t>Hilda</t>
+  </si>
+  <si>
+    <t>Oneill</t>
+  </si>
+  <si>
+    <t>Ori</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Xandra</t>
+  </si>
+  <si>
+    <t>Cardenas</t>
   </si>
 </sst>
 </file>
@@ -2892,7 +3183,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2946,12 +3237,13 @@
     <xf numFmtId="21" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3476,6 +3768,131 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flowchart: Alternate Process 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10B4C220-3877-4510-9540-6AAED6FA9BBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11620500" y="238125"/>
+          <a:ext cx="3267075" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Get the name of the Departement in Column in column E using Vlookup with the help of column G and H.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4681,7 +5098,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> funtion</a:t>
+            <a:t> formula</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-IN" sz="1100">
@@ -4696,7 +5113,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> and extract</a:t>
+            <a:t> in column D and E to extract</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-IN" sz="1100" baseline="0">
@@ -4711,7 +5128,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> first name and last name in column D and E respectively.</a:t>
+            <a:t> first name and last name from column A and B.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4745,7 +5162,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>2) using the results in column D and E. Get the Full name in colum F</a:t>
+            <a:t>2) Using the results in column D and E. Get the Full name in colum F</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4766,6 +5183,489 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
+          <a:endParaRPr lang="en-IN">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flowchart: Alternate Process 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B5102CB-723B-492A-81EB-0F16D0458CC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14268450" y="1181099"/>
+          <a:ext cx="3219449" cy="1304925"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Get Email ID in column D in the below format</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          firstname.lastname@company.com</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IN">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>2) Remove .</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> character from phone number Column E and convert to number format</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IN" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>3) Get years of experience in column K or L using hire date</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flowchart: Alternate Process 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F3192A4-A4E9-4FB0-9951-C39FA9882F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9391651" y="247651"/>
+          <a:ext cx="3771900" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Convert the given data into a table and try all the funtions that we did eariler and note down the differences.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2790825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flowchart: Alternate Process 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F063C525-034F-4DEF-B778-E6A030FFBBDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9782175" y="2838450"/>
+          <a:ext cx="3267075" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> For the given Rank in cell B15 get all the details from the table using VlookUp.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-IN">
             <a:ln>
               <a:noFill/>
@@ -5417,15 +6317,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2151C0B-73BA-4D05-A62D-E4D9FD47320B}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -5704,10 +6604,6 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I14" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -5716,44 +6612,59 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I15" s="2" t="s">
+      <c r="A15" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I16" s="2" t="s">
+      <c r="B16" s="45"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="2" t="s">
+      <c r="B17" s="45"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="2" t="s">
+      <c r="B18" s="51"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="2" t="s">
+      <c r="B19" s="45"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="2" t="s">
+      <c r="B20" s="45"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="2" t="s">
+      <c r="B21" s="45"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>270</v>
       </c>
+      <c r="B22" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5762,7 +6673,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:I21"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6080,7 +6991,7 @@
   <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6089,7 +7000,7 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -6097,20 +7008,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="E1" t="s">
-        <v>841</v>
+      <c r="E1" s="2" t="s">
+        <v>717</v>
       </c>
       <c r="G1" t="s">
         <v>388</v>
@@ -7782,6 +8693,8 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7790,7 +8703,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8132,7 +9045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B59B5EA-5F36-4506-9B80-2736CCDF45D1}">
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -11092,10 +12005,10 @@
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1"/>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="49" t="s">
         <v>304</v>
       </c>
-      <c r="D1" s="47"/>
+      <c r="D1" s="49"/>
       <c r="E1"/>
       <c r="F1" s="2" t="s">
         <v>310</v>
@@ -11172,7 +12085,7 @@
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
-      <c r="M4" s="48"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -11471,34 +12384,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="P1" s="14" t="s">
@@ -11533,9 +12446,9 @@
       <c r="G2" s="16">
         <v>70</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
       <c r="S2" t="s">
         <v>305</v>
       </c>
@@ -11562,9 +12475,9 @@
       <c r="G3" s="16">
         <v>73</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
       <c r="S3" t="s">
         <v>306</v>
       </c>
@@ -11591,9 +12504,9 @@
       <c r="G4" s="16">
         <v>72</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
@@ -11617,9 +12530,9 @@
       <c r="G5" s="16">
         <v>77</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>114</v>
       </c>
@@ -11652,9 +12565,9 @@
       <c r="G6" s="16">
         <v>53</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
       <c r="P6" s="4" t="s">
         <v>119</v>
       </c>
@@ -11683,9 +12596,9 @@
       <c r="G7" s="16">
         <v>92</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
       <c r="P7" s="4" t="s">
         <v>124</v>
       </c>
@@ -11714,9 +12627,9 @@
       <c r="G8" s="16">
         <v>89</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
       <c r="P8" s="4" t="s">
         <v>129</v>
       </c>
@@ -11745,9 +12658,9 @@
       <c r="G9" s="16">
         <v>86</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
     </row>
     <row r="10" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
@@ -11771,9 +12684,9 @@
       <c r="G10" s="16">
         <v>92</v>
       </c>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
@@ -11798,9 +12711,9 @@
       <c r="G11" s="16">
         <v>68</v>
       </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
     </row>
     <row r="12" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
@@ -11824,9 +12737,9 @@
       <c r="G12" s="16">
         <v>79</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
     </row>
     <row r="13" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -11850,9 +12763,9 @@
       <c r="G13" s="16">
         <v>41</v>
       </c>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
     </row>
     <row r="14" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
@@ -11876,9 +12789,9 @@
       <c r="G14" s="16">
         <v>97</v>
       </c>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
     </row>
     <row r="15" spans="1:19" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
@@ -11902,9 +12815,9 @@
       <c r="G15" s="16">
         <v>78</v>
       </c>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -11932,9 +12845,9 @@
       <c r="G16" s="16">
         <v>61</v>
       </c>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
     </row>
     <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
@@ -11958,9 +12871,9 @@
       <c r="G17" s="16">
         <v>51</v>
       </c>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
@@ -11984,9 +12897,9 @@
       <c r="G18" s="16">
         <v>39</v>
       </c>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
@@ -12010,9 +12923,9 @@
       <c r="G19" s="16">
         <v>98</v>
       </c>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
@@ -12036,9 +12949,9 @@
       <c r="G20" s="16">
         <v>77</v>
       </c>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
@@ -12062,9 +12975,9 @@
       <c r="G21" s="16">
         <v>46</v>
       </c>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
@@ -12088,9 +13001,9 @@
       <c r="G22" s="16">
         <v>41</v>
       </c>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
     </row>
     <row r="23" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
@@ -12114,9 +13027,9 @@
       <c r="G23" s="16">
         <v>94</v>
       </c>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
@@ -12140,9 +13053,9 @@
       <c r="G24" s="16">
         <v>50</v>
       </c>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
@@ -12166,9 +13079,9 @@
       <c r="G25" s="16">
         <v>78</v>
       </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
     </row>
     <row r="26" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
@@ -12192,9 +13105,9 @@
       <c r="G26" s="16">
         <v>95</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
     </row>
     <row r="27" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
@@ -12218,9 +13131,9 @@
       <c r="G27" s="16">
         <v>99</v>
       </c>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
     </row>
     <row r="28" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
@@ -12244,9 +13157,9 @@
       <c r="G28" s="16">
         <v>55</v>
       </c>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
     </row>
     <row r="29" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
@@ -12270,9 +13183,9 @@
       <c r="G29" s="16">
         <v>80</v>
       </c>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
     </row>
     <row r="30" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
@@ -12296,9 +13209,9 @@
       <c r="G30" s="16">
         <v>71</v>
       </c>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
     </row>
     <row r="31" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
@@ -12322,9 +13235,9 @@
       <c r="G31" s="16">
         <v>47</v>
       </c>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
     </row>
     <row r="32" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
@@ -12348,9 +13261,9 @@
       <c r="G32" s="16">
         <v>78</v>
       </c>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
     </row>
     <row r="33" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
@@ -12374,9 +13287,9 @@
       <c r="G33" s="16">
         <v>83</v>
       </c>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
     </row>
     <row r="34" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
@@ -12400,9 +13313,9 @@
       <c r="G34" s="16">
         <v>65</v>
       </c>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
     </row>
     <row r="35" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
@@ -12426,9 +13339,9 @@
       <c r="G35" s="16">
         <v>65</v>
       </c>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
     </row>
     <row r="36" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
@@ -12452,9 +13365,9 @@
       <c r="G36" s="16">
         <v>94</v>
       </c>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
@@ -12478,9 +13391,9 @@
       <c r="G37" s="16">
         <v>87</v>
       </c>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
     </row>
     <row r="38" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
@@ -12504,9 +13417,9 @@
       <c r="G38" s="16">
         <v>75</v>
       </c>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
     </row>
     <row r="39" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
@@ -12530,9 +13443,9 @@
       <c r="G39" s="16">
         <v>62</v>
       </c>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
@@ -12556,9 +13469,9 @@
       <c r="G40" s="16">
         <v>63</v>
       </c>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
     </row>
     <row r="41" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
@@ -12582,9 +13495,9 @@
       <c r="G41" s="16">
         <v>75</v>
       </c>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="50"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
     </row>
     <row r="42" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
@@ -12608,9 +13521,9 @@
       <c r="G42" s="16">
         <v>72</v>
       </c>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
@@ -12634,9 +13547,9 @@
       <c r="G43" s="16">
         <v>67</v>
       </c>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="16" t="s">
@@ -12660,9 +13573,9 @@
       <c r="G44" s="16">
         <v>83</v>
       </c>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
     </row>
     <row r="45" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
@@ -12686,9 +13599,9 @@
       <c r="G45" s="16">
         <v>87</v>
       </c>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
@@ -12712,9 +13625,9 @@
       <c r="G46" s="16">
         <v>88</v>
       </c>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
@@ -12738,9 +13651,9 @@
       <c r="G47" s="16">
         <v>80</v>
       </c>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
     </row>
     <row r="48" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
@@ -12764,9 +13677,9 @@
       <c r="G48" s="16">
         <v>82</v>
       </c>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
     </row>
     <row r="49" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
@@ -12790,9 +13703,9 @@
       <c r="G49" s="16">
         <v>80</v>
       </c>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
     </row>
     <row r="50" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
@@ -12816,9 +13729,9 @@
       <c r="G50" s="16">
         <v>56</v>
       </c>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="48"/>
     </row>
     <row r="51" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
@@ -12842,9 +13755,9 @@
       <c r="G51" s="16">
         <v>76</v>
       </c>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -13132,7 +14045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BBF5D9-8FB7-42E4-B0A4-B8AC86EC7EE1}">
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13252,7 +14167,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B6" t="s">
         <v>135</v>
@@ -13317,7 +14232,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="N10" s="40" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -13331,7 +14246,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="N11" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -13345,7 +14260,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="N12" s="4" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -13359,7 +14274,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="N13" s="4" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -13373,7 +14288,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="N14" s="4" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -13387,17 +14302,17 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="N15" s="4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="N16" s="4" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="17" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N17" s="4" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
   </sheetData>
@@ -13412,7 +14327,7 @@
   <dimension ref="A1:AH9097"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13473,16 +14388,16 @@
         <v>389</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>852</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>853</v>
-      </c>
       <c r="O1" s="4" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="V1" s="4"/>
       <c r="AB1" s="2"/>
@@ -13523,11 +14438,11 @@
       <c r="K2" s="45"/>
       <c r="L2" s="45"/>
       <c r="N2" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="O2" s="38">
         <f ca="1">TODAY()</f>
-        <v>45018</v>
+        <v>45019</v>
       </c>
       <c r="V2" s="4"/>
     </row>
@@ -16731,6 +17646,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16760,7 +17676,7 @@
         <v>329</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -16769,7 +17685,7 @@
       </c>
       <c r="B2" s="32">
         <f ca="1">TODAY()</f>
-        <v>45018</v>
+        <v>45019</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>331</v>
@@ -16781,7 +17697,7 @@
       </c>
       <c r="B3" s="34">
         <f ca="1">NOW()</f>
-        <v>45018.805527777775</v>
+        <v>45019.242861226849</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>333</v>
@@ -16817,7 +17733,7 @@
       </c>
       <c r="B6" s="33">
         <f ca="1">DAY(B2)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="33" t="s">
         <v>339</v>
@@ -16829,7 +17745,7 @@
       </c>
       <c r="B7" s="33">
         <f ca="1">HOUR(B3)</f>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>341</v>
@@ -16841,7 +17757,7 @@
       </c>
       <c r="B8" s="33">
         <f ca="1">MINUTE(B3)</f>
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>343</v>
@@ -16853,7 +17769,7 @@
       </c>
       <c r="B9" s="33">
         <f ca="1">SECOND(B3)</f>
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>345</v>
@@ -16865,7 +17781,7 @@
       </c>
       <c r="B10" s="32">
         <f ca="1">EDATE(B2,B5)</f>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>347</v>
@@ -16895,7 +17811,7 @@
         <v>351</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -16910,7 +17826,7 @@
         <v>353</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -16919,7 +17835,7 @@
       </c>
       <c r="B14" s="32">
         <f ca="1">WORKDAY(B2,B6)</f>
-        <v>45020</v>
+        <v>45022</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>355</v>
@@ -16931,7 +17847,7 @@
       </c>
       <c r="B15" s="32">
         <f ca="1">WORKDAY.INTL(B2,B6,1)</f>
-        <v>45020</v>
+        <v>45022</v>
       </c>
       <c r="C15" s="33" t="s">
         <v>357</v>
@@ -16943,7 +17859,7 @@
       </c>
       <c r="B16" s="33">
         <f ca="1">NETWORKDAYS(B2,B10)</f>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>359</v>
@@ -16955,7 +17871,7 @@
       </c>
       <c r="B17" s="33">
         <f ca="1">NETWORKDAYS.INTL(B2,B10,1)</f>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>361</v>
@@ -16967,7 +17883,7 @@
       </c>
       <c r="B18" s="36">
         <f ca="1">DATE(B4,B5,B6)</f>
-        <v>45018</v>
+        <v>45019</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>363</v>
@@ -16979,7 +17895,7 @@
       </c>
       <c r="B19" s="37">
         <f ca="1">TIME(B7,B8,B9)</f>
-        <v>0.80553240740740739</v>
+        <v>0.24285879629629628</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>365</v>
@@ -16991,7 +17907,7 @@
       </c>
       <c r="B20" s="33">
         <f ca="1">WEEKDAY(B2,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>367</v>
@@ -17003,7 +17919,7 @@
       </c>
       <c r="B21" s="33">
         <f ca="1">WEEKDAY(B2,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>367</v>
@@ -17039,7 +17955,7 @@
       </c>
       <c r="B24" s="33">
         <f ca="1">DATEDIF(B2,B11,"D")</f>
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C24" s="33" t="s">
         <v>374</v>
@@ -17079,1193 +17995,1350 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4979C08-6F67-4EBD-8816-064FDFF2B18B}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>859</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>858</v>
       </c>
       <c r="C1" t="s">
+        <v>860</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="50" t="s">
+        <v>483</v>
+      </c>
+      <c r="C2" t="s">
+        <v>861</v>
+      </c>
+      <c r="D2">
         <v>77</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>64</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>95</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>84</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="50" t="s">
+        <v>862</v>
+      </c>
+      <c r="C3" t="s">
+        <v>863</v>
+      </c>
+      <c r="D3">
         <v>88</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>90</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>86</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>94</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="50" t="s">
+        <v>864</v>
+      </c>
+      <c r="C4" t="s">
+        <v>865</v>
+      </c>
+      <c r="D4">
         <v>84</v>
-      </c>
-      <c r="D4">
-        <v>69</v>
       </c>
       <c r="E4">
         <v>69</v>
       </c>
       <c r="F4">
+        <v>69</v>
+      </c>
+      <c r="G4">
         <v>53</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="50" t="s">
+        <v>866</v>
+      </c>
+      <c r="C5" t="s">
+        <v>867</v>
+      </c>
+      <c r="D5">
         <v>40</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>45</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>83</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>75</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="50" t="s">
+        <v>868</v>
+      </c>
+      <c r="C6" t="s">
+        <v>869</v>
+      </c>
+      <c r="D6">
         <v>47</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>70</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>48</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>52</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="50" t="s">
+        <v>870</v>
+      </c>
+      <c r="C7" t="s">
+        <v>871</v>
+      </c>
+      <c r="D7">
         <v>95</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>82</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>40</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>81</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="50" t="s">
+        <v>872</v>
+      </c>
+      <c r="C8" t="s">
+        <v>873</v>
+      </c>
+      <c r="D8">
         <v>78</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>95</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>60</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>85</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="50" t="s">
+        <v>874</v>
+      </c>
+      <c r="C9" t="s">
+        <v>875</v>
+      </c>
+      <c r="D9">
         <v>97</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>48</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>76</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>98</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="50" t="s">
+        <v>876</v>
+      </c>
+      <c r="C10" t="s">
+        <v>877</v>
+      </c>
+      <c r="D10">
         <v>62</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>45</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>91</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>88</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="50" t="s">
+        <v>878</v>
+      </c>
+      <c r="C11" t="s">
+        <v>879</v>
+      </c>
+      <c r="D11">
         <v>45</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>59</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>69</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>47</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="50" t="s">
+        <v>880</v>
+      </c>
+      <c r="C12" t="s">
+        <v>881</v>
+      </c>
+      <c r="D12">
         <v>51</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>45</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>84</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>93</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="50" t="s">
+        <v>427</v>
+      </c>
+      <c r="C13" t="s">
+        <v>882</v>
+      </c>
+      <c r="D13">
         <v>84</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>60</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>45</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>20</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="50" t="s">
+        <v>883</v>
+      </c>
+      <c r="C14" t="s">
+        <v>884</v>
+      </c>
+      <c r="D14">
         <v>90</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>63</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>66</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>47</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="50" t="s">
+        <v>885</v>
+      </c>
+      <c r="C15" t="s">
+        <v>886</v>
+      </c>
+      <c r="D15">
         <v>86</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>63</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>56</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>45</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="50" t="s">
+        <v>887</v>
+      </c>
+      <c r="C16" t="s">
+        <v>888</v>
+      </c>
+      <c r="D16">
         <v>75</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>81</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>70</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>72</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="50" t="s">
+        <v>889</v>
+      </c>
+      <c r="C17" t="s">
+        <v>890</v>
+      </c>
+      <c r="D17">
         <v>35</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>76</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>98</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>66</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="50" t="s">
+        <v>891</v>
+      </c>
+      <c r="C18" t="s">
+        <v>892</v>
+      </c>
+      <c r="D18">
         <v>53</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>65</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>79</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>53</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="50" t="s">
+        <v>893</v>
+      </c>
+      <c r="C19" t="s">
+        <v>894</v>
+      </c>
+      <c r="D19">
         <v>85</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>88</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>100</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>92</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="50" t="s">
+        <v>895</v>
+      </c>
+      <c r="C20" t="s">
+        <v>896</v>
+      </c>
+      <c r="D20">
         <v>89</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>91</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>89</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>84</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21">
-        <v>78</v>
+      <c r="B21" s="50" t="s">
+        <v>897</v>
+      </c>
+      <c r="C21" t="s">
+        <v>898</v>
       </c>
       <c r="D21">
         <v>78</v>
       </c>
       <c r="E21">
+        <v>78</v>
+      </c>
+      <c r="F21">
         <v>85</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>47</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="50" t="s">
+        <v>899</v>
+      </c>
+      <c r="C22" t="s">
+        <v>900</v>
+      </c>
+      <c r="D22">
         <v>20</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>57</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>88</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>70</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="50" t="s">
+        <v>615</v>
+      </c>
+      <c r="C23" t="s">
+        <v>901</v>
+      </c>
+      <c r="D23">
+        <v>65</v>
+      </c>
+      <c r="E23">
+        <v>55</v>
+      </c>
+      <c r="F23">
         <v>53</v>
       </c>
-      <c r="C23">
-        <v>65</v>
-      </c>
-      <c r="D23">
-        <v>55</v>
-      </c>
-      <c r="E23">
-        <v>53</v>
-      </c>
-      <c r="F23">
+      <c r="G23">
         <v>75</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="50" t="s">
+        <v>902</v>
+      </c>
+      <c r="C24" t="s">
+        <v>903</v>
+      </c>
+      <c r="D24">
         <v>53</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>92</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>91</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>48</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="50" t="s">
+        <v>904</v>
+      </c>
+      <c r="C25" t="s">
+        <v>905</v>
+      </c>
+      <c r="D25">
         <v>68</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>53</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>38</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>85</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="50" t="s">
+        <v>906</v>
+      </c>
+      <c r="C26" t="s">
+        <v>907</v>
+      </c>
+      <c r="D26">
         <v>82</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>99</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>88</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>98</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="50" t="s">
+        <v>908</v>
+      </c>
+      <c r="C27" t="s">
+        <v>909</v>
+      </c>
+      <c r="D27">
         <v>73</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>50</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>73</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>43</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>62</v>
       </c>
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="50" t="s">
+        <v>910</v>
+      </c>
+      <c r="C28" t="s">
+        <v>911</v>
+      </c>
+      <c r="D28">
         <v>93</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>95</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>49</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>47</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="50" t="s">
+        <v>912</v>
+      </c>
+      <c r="C29" t="s">
+        <v>913</v>
+      </c>
+      <c r="D29">
         <v>84</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>92</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>93</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>95</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
-      <c r="B30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="50" t="s">
+        <v>914</v>
+      </c>
+      <c r="C30" t="s">
+        <v>915</v>
+      </c>
+      <c r="D30">
         <v>75</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>91</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>68</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>75</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
-      <c r="B31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="50" t="s">
+        <v>916</v>
+      </c>
+      <c r="C31" t="s">
+        <v>917</v>
+      </c>
+      <c r="D31">
         <v>82</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>89</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>57</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>43</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="50" t="s">
+        <v>918</v>
+      </c>
+      <c r="C32" t="s">
+        <v>919</v>
+      </c>
+      <c r="D32">
         <v>72</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>99</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>78</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>92</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
-      <c r="B33" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="50" t="s">
+        <v>920</v>
+      </c>
+      <c r="C33" t="s">
+        <v>921</v>
+      </c>
+      <c r="D33">
         <v>89</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>93</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>68</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>93</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
-      <c r="B34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="50" t="s">
+        <v>922</v>
+      </c>
+      <c r="C34" t="s">
+        <v>923</v>
+      </c>
+      <c r="D34">
         <v>69</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>67</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>99</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>74</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
-      <c r="B35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35">
+      <c r="B35" s="50" t="s">
+        <v>924</v>
+      </c>
+      <c r="C35" t="s">
+        <v>903</v>
+      </c>
+      <c r="D35">
         <v>82</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>72</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>98</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>75</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>78</v>
       </c>
-      <c r="B36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36">
+      <c r="B36" s="50" t="s">
+        <v>925</v>
+      </c>
+      <c r="C36" t="s">
+        <v>391</v>
+      </c>
+      <c r="D36">
         <v>92</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>84</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>32</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>93</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
-      <c r="B37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37">
+      <c r="B37" s="50" t="s">
+        <v>926</v>
+      </c>
+      <c r="C37" t="s">
+        <v>927</v>
+      </c>
+      <c r="D37">
         <v>97</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>82</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>62</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>90</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>82</v>
       </c>
-      <c r="B38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38">
+      <c r="B38" s="50" t="s">
+        <v>928</v>
+      </c>
+      <c r="C38" t="s">
+        <v>929</v>
+      </c>
+      <c r="D38">
         <v>66</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>86</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>61</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>71</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
-      <c r="B39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39">
+      <c r="B39" s="50" t="s">
+        <v>930</v>
+      </c>
+      <c r="C39" t="s">
+        <v>931</v>
+      </c>
+      <c r="D39">
         <v>65</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>92</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>88</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>63</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>86</v>
       </c>
-      <c r="B40" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40">
+      <c r="B40" s="50" t="s">
+        <v>932</v>
+      </c>
+      <c r="C40" t="s">
+        <v>933</v>
+      </c>
+      <c r="D40">
         <v>70</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>95</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>96</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>85</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="50" t="s">
+        <v>934</v>
+      </c>
+      <c r="C41" t="s">
+        <v>935</v>
+      </c>
+      <c r="D41">
         <v>68</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>75</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>94</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>93</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
-      <c r="B42" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42">
+      <c r="B42" s="50" t="s">
+        <v>936</v>
+      </c>
+      <c r="C42" t="s">
+        <v>937</v>
+      </c>
+      <c r="D42">
         <v>98</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>64</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>100</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>64</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
-      <c r="B43" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43">
+      <c r="B43" s="50" t="s">
+        <v>938</v>
+      </c>
+      <c r="C43" t="s">
+        <v>939</v>
+      </c>
+      <c r="D43">
         <v>32</v>
-      </c>
-      <c r="D43">
-        <v>80</v>
       </c>
       <c r="E43">
         <v>80</v>
       </c>
       <c r="F43">
+        <v>80</v>
+      </c>
+      <c r="G43">
         <v>77</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>94</v>
       </c>
-      <c r="B44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44">
+      <c r="B44" s="50" t="s">
+        <v>940</v>
+      </c>
+      <c r="C44" t="s">
+        <v>941</v>
+      </c>
+      <c r="D44">
         <v>85</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>71</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>86</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>65</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45">
+      <c r="B45" s="50" t="s">
+        <v>942</v>
+      </c>
+      <c r="C45" t="s">
+        <v>943</v>
+      </c>
+      <c r="D45">
         <v>87</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>84</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>78</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>65</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>98</v>
       </c>
-      <c r="B46" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46">
+      <c r="B46" s="50" t="s">
+        <v>944</v>
+      </c>
+      <c r="C46" t="s">
+        <v>945</v>
+      </c>
+      <c r="D46">
         <v>94</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>79</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>73</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>62</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>100</v>
       </c>
-      <c r="B47" t="s">
-        <v>101</v>
-      </c>
-      <c r="C47">
+      <c r="B47" s="50" t="s">
+        <v>946</v>
+      </c>
+      <c r="C47" t="s">
+        <v>947</v>
+      </c>
+      <c r="D47">
         <v>77</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>76</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>72</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>77</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>102</v>
       </c>
-      <c r="B48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48">
+      <c r="B48" s="50" t="s">
+        <v>948</v>
+      </c>
+      <c r="C48" t="s">
+        <v>949</v>
+      </c>
+      <c r="D48">
         <v>85</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>98</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>82</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>99</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>104</v>
       </c>
-      <c r="B49" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49">
+      <c r="B49" s="50" t="s">
+        <v>950</v>
+      </c>
+      <c r="C49" t="s">
+        <v>951</v>
+      </c>
+      <c r="D49">
         <v>65</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>90</v>
-      </c>
-      <c r="E49">
-        <v>73</v>
       </c>
       <c r="F49">
         <v>73</v>
       </c>
       <c r="G49">
+        <v>73</v>
+      </c>
+      <c r="H49">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>106</v>
       </c>
-      <c r="B50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50">
+      <c r="B50" s="50" t="s">
+        <v>952</v>
+      </c>
+      <c r="C50" t="s">
+        <v>953</v>
+      </c>
+      <c r="D50">
         <v>45</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>66</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>70</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>31</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>108</v>
       </c>
-      <c r="B51" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51">
+      <c r="B51" s="50" t="s">
+        <v>954</v>
+      </c>
+      <c r="C51" t="s">
+        <v>955</v>
+      </c>
+      <c r="D51">
         <v>61</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>93</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>80</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>60</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>